<commit_message>
new local strings added
</commit_message>
<xml_diff>
--- a/src/TestOkur.WebApi/Application/Localization/tr.xlsx
+++ b/src/TestOkur.WebApi/Application/Localization/tr.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
   <si>
     <t>Ad</t>
   </si>
@@ -479,6 +479,18 @@
   </si>
   <si>
     <t>Tum formlar tarandi</t>
+  </si>
+  <si>
+    <t>MigrationQuestionPrompt</t>
+  </si>
+  <si>
+    <t>Eski uygulamadaki öğrenci verilerinizi giriş ekranındakı 'Eski Sistem Verilerini Aktar' butonunu kullanabilirsiniz.</t>
+  </si>
+  <si>
+    <t>UserExpired</t>
+  </si>
+  <si>
+    <t>Kullanıcı hesabınızın süresi dolmuştur. TestOkur'u kullanmaya devam etmek için  web sitemizden lisans yenileme işlemi yapmalısınız</t>
   </si>
 </sst>
 </file>
@@ -745,7 +757,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="34.43"/>
-    <col customWidth="1" min="2" max="2" width="83.0"/>
+    <col customWidth="1" min="2" max="2" width="116.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1372,6 +1384,22 @@
         <v>155</v>
       </c>
     </row>
+    <row r="79">
+      <c r="A79" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Missing local string added
</commit_message>
<xml_diff>
--- a/src/TestOkur.WebApi/Application/Localization/tr.xlsx
+++ b/src/TestOkur.WebApi/Application/Localization/tr.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="162">
   <si>
     <t>Ad</t>
   </si>
@@ -491,6 +491,12 @@
   </si>
   <si>
     <t>Kullanıcı hesabınızın süresi dolmuştur. TestOkur'u kullanmaya devam etmek için  web sitemizden lisans yenileme işlemi yapmalısınız</t>
+  </si>
+  <si>
+    <t>UserNotActive</t>
+  </si>
+  <si>
+    <t>Kullanıcı hesabınız aktif değildir. Lütfen TestOkur yetkilileri ile görüşünüz</t>
   </si>
 </sst>
 </file>
@@ -1400,6 +1406,14 @@
         <v>159</v>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Online user tracking added
</commit_message>
<xml_diff>
--- a/src/TestOkur.WebApi/Application/Localization/tr.xlsx
+++ b/src/TestOkur.WebApi/Application/Localization/tr.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="176">
   <si>
     <t>Ad</t>
   </si>
@@ -533,6 +533,12 @@
   </si>
   <si>
     <t>Sadece sinif ve ogrenci bilgileri aktarilacaktir. Eski  sinav ve optik formlar yeni sistemle uyumlu olmadigi icin bunlar aktarilmayacaktir.</t>
+  </si>
+  <si>
+    <t>ESchoolLoginWarning</t>
+  </si>
+  <si>
+    <t>E-Okul'dan veri cekilmesi esnasinda kullandiginiz kullanici bilgieri ile baska bir yerde oturum acmamaniz gerekmektedir. Oturum acildigi takdir de  uygulamadaki  veri aktarimi kesilecektir ve islem devam etmeyecektir.</t>
   </si>
 </sst>
 </file>
@@ -1498,6 +1504,14 @@
         <v>173</v>
       </c>
     </row>
+    <row r="88">
+      <c r="A88" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
PasswordResetUserNotFound custom error message
</commit_message>
<xml_diff>
--- a/src/TestOkur.WebApi/Application/Localization/tr.xlsx
+++ b/src/TestOkur.WebApi/Application/Localization/tr.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="180">
   <si>
     <t>Ad</t>
   </si>
@@ -545,6 +545,12 @@
   </si>
   <si>
     <t>Optik form yazdirmak istediginz sinif(lar)da  ogrenci bulunamadi.</t>
+  </si>
+  <si>
+    <t>PasswordResetUserNotFound</t>
+  </si>
+  <si>
+    <t>Bu e-posta adresine ait kullanici kaydi bulunmamistir. Lutfen e-posta adresinizin dogru oldugundan emin olunuz.</t>
   </si>
 </sst>
 </file>
@@ -1526,6 +1532,14 @@
         <v>177</v>
       </c>
     </row>
+    <row r="90">
+      <c r="A90" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Missing local string for InsufficientFunds added
</commit_message>
<xml_diff>
--- a/src/TestOkur.WebApi/Application/Localization/tr.xlsx
+++ b/src/TestOkur.WebApi/Application/Localization/tr.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
   <si>
     <t>Ad</t>
   </si>
@@ -551,6 +551,12 @@
   </si>
   <si>
     <t>Bu e-posta adresine ait kullanici kaydi bulunmamistir. Lutfen e-posta adresinizin dogru oldugundan emin olunuz.</t>
+  </si>
+  <si>
+    <t>InsufficientFunds</t>
+  </si>
+  <si>
+    <t>SMS bakiyeniz yetersizdir.</t>
   </si>
 </sst>
 </file>
@@ -1540,6 +1546,14 @@
         <v>179</v>
       </c>
     </row>
+    <row r="91">
+      <c r="A91" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Missing local strings added
</commit_message>
<xml_diff>
--- a/src/TestOkur.WebApi/Application/Localization/tr.xlsx
+++ b/src/TestOkur.WebApi/Application/Localization/tr.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="192">
   <si>
     <t>Ad</t>
   </si>
@@ -575,6 +575,18 @@
   </si>
   <si>
     <t>Lutfen mesaj gonderilecek olan telefon numaralarini giriniz.</t>
+  </si>
+  <si>
+    <t>Lutfen E-Posta Giriniz</t>
+  </si>
+  <si>
+    <t>Lutfen Parola Giriniz</t>
+  </si>
+  <si>
+    <t>invalid_grant</t>
+  </si>
+  <si>
+    <t>Gecersiz kullanici adi veya parola</t>
   </si>
 </sst>
 </file>
@@ -1596,6 +1608,30 @@
         <v>187</v>
       </c>
     </row>
+    <row r="95">
+      <c r="A95" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
new local string added
</commit_message>
<xml_diff>
--- a/src/TestOkur.WebApi/Application/Localization/tr.xlsx
+++ b/src/TestOkur.WebApi/Application/Localization/tr.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
   <si>
     <t>Ad</t>
   </si>
@@ -593,6 +593,12 @@
   </si>
   <si>
     <t>Ortak deneme sinavlari sadece  TestOkur yoneticileri tarafindan silinebilir.</t>
+  </si>
+  <si>
+    <t>StudentOpticalFormGradeMismatch</t>
+  </si>
+  <si>
+    <t>En son okunan optik form  ile ondan once okunan optik form farkli siniflara ait. Bu gibi durumlar raporlardaki ortalama ve siralamayi etkileyebilir.</t>
   </si>
 </sst>
 </file>
@@ -1638,6 +1644,14 @@
         <v>193</v>
       </c>
     </row>
+    <row r="98">
+      <c r="A98" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>